<commit_message>
Add Wilcox test of MOI by Region (with Bonferroni)
</commit_message>
<xml_diff>
--- a/CSP-MSP1_Comparison/MSP-CSP_mMOI_Comparison.xlsx
+++ b/CSP-MSP1_Comparison/MSP-CSP_mMOI_Comparison.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\HaplotypR_tests\MSP-CSP_Diversity\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\Ghana_CSP_Haplotypes\CSP-MSP1_Comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167936CF-DA5A-4D8D-91D0-9F3BFB50EC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7315EA22-0033-4D32-B85B-E01C7E9B5598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{CAD903C9-5812-4A89-B6BA-C1BBD4A709E4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="1" activeTab="3" xr2:uid="{CAD903C9-5812-4A89-B6BA-C1BBD4A709E4}"/>
   </bookViews>
   <sheets>
     <sheet name="All CSP &amp; MSP Haplotypes" sheetId="2" r:id="rId1"/>
     <sheet name="Pivot" sheetId="4" r:id="rId2"/>
     <sheet name="Pivot_raw" sheetId="6" r:id="rId3"/>
+    <sheet name="Wilcox" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'All CSP &amp; MSP Haplotypes'!$A$1:$D$446</definedName>
@@ -23,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2060" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2066" uniqueCount="330">
   <si>
     <t>SampleID</t>
   </si>
@@ -1015,6 +1016,24 @@
   </si>
   <si>
     <t>Central</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t>Comparison</t>
+  </si>
+  <si>
+    <t>North vs. Central</t>
+  </si>
+  <si>
+    <t>South vs. Central</t>
+  </si>
+  <si>
+    <t>South vs. North</t>
+  </si>
+  <si>
+    <t>*with Bonferroni</t>
   </si>
 </sst>
 </file>
@@ -3892,7 +3911,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BCCE6568-57F3-4A6B-8007-5E29808B5353}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{BCCE6568-57F3-4A6B-8007-5E29808B5353}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:C93" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField compact="0" outline="0" showAll="0"/>
@@ -11860,8 +11879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69F3A14-78EA-40D8-B3C0-5B5011CD278C}">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13136,4 +13155,60 @@
   <autoFilter ref="A1:C90" xr:uid="{FBB31559-081C-43AB-9829-636C7A1D5347}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D379280-2DC8-48D4-921B-126BD5D9308E}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B2">
+        <v>0.29185544000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B3">
+        <v>8.9511080000000007E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>